<commit_message>
updated example DR profile
</commit_message>
<xml_diff>
--- a/docs/example-dr.xlsx
+++ b/docs/example-dr.xlsx
@@ -595,7 +595,7 @@
     <t>DocumentReference.author</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/StructureDefinition/Practitioner], CanonicalType[http://hl7.org/fhir/StructureDefinition/Organization], CanonicalType[http://hl7.org/fhir/StructureDefinition/Device], CanonicalType[http://hl7.org/fhir/StructureDefinition/Patient], CanonicalType[http://hl7.org/fhir/StructureDefinition/RelatedPerson]]}
+    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/us/core/StructureDefinition/us-core-organization], CanonicalType[http://hl7.org/fhir/us/core/StructureDefinition/us-core-practitioner], CanonicalType[http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient], CanonicalType[http://hl7.org/fhir/StructureDefinition/Device], CanonicalType[http://hl7.org/fhir/StructureDefinition/RelatedPerson]]}
 </t>
   </si>
   <si>
@@ -3611,7 +3611,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="20" hidden="true">
+    <row r="20">
       <c r="A20" t="s" s="2">
         <v>185</v>
       </c>
@@ -3621,13 +3621,13 @@
       </c>
       <c r="D20" s="2"/>
       <c r="E20" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F20" t="s" s="2">
         <v>42</v>
       </c>
       <c r="G20" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H20" t="s" s="2">
         <v>40</v>

</xml_diff>